<commit_message>
update Cold/Hot mold class
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -56,14 +56,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjGGN4kE1m1trTycLFU0hgTtXNLrQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi4LXIZBHotTYflY+ty8QSYWHj1aQ=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="210">
   <si>
     <t>項次</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>到廠時間</t>
+  </si>
+  <si>
+    <t>膜腔數</t>
   </si>
   <si>
     <t>翻修日期</t>
@@ -2968,7 +2971,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="82" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="70" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -37567,18 +37570,20 @@
       <c r="C2" s="196" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="197"/>
+      <c r="D2" s="197" t="s">
+        <v>162</v>
+      </c>
       <c r="E2" s="198" t="s">
         <v>97</v>
       </c>
       <c r="F2" s="199" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G2" s="200" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H2" s="201" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" ht="16.5" hidden="1" customHeight="1">
@@ -37589,7 +37594,7 @@
         <v>1996.8</v>
       </c>
       <c r="C3" s="204" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D3" s="205">
         <v>48.0</v>
@@ -37598,13 +37603,13 @@
         <v>48.0</v>
       </c>
       <c r="F3" s="207" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G3" s="208">
         <v>100739.0</v>
       </c>
       <c r="H3" s="209" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" ht="16.5" hidden="1" customHeight="1">
@@ -37625,12 +37630,12 @@
         <v>1996.4</v>
       </c>
       <c r="C5" s="214" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="153" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G5" s="215">
         <v>100403.0</v>
@@ -37650,7 +37655,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="153" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G6" s="215">
         <v>394212.0</v>
@@ -37665,12 +37670,12 @@
         <v>1997.5</v>
       </c>
       <c r="C7" s="214" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="153" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G7" s="215">
         <v>102099.0</v>
@@ -37690,11 +37695,11 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="156" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G8" s="215"/>
       <c r="H8" s="221" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" ht="16.5" customHeight="1">
@@ -37710,7 +37715,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="224" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G9" s="225">
         <v>432686.0</v>
@@ -37730,7 +37735,7 @@
       <c r="D10" s="116"/>
       <c r="E10" s="11"/>
       <c r="F10" s="182" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G10" s="229">
         <v>418013.0</v>
@@ -37745,7 +37750,7 @@
         <v>2004.12</v>
       </c>
       <c r="C11" s="233" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D11" s="149">
         <v>72.0</v>
@@ -37754,10 +37759,10 @@
         <v>25</v>
       </c>
       <c r="F11" s="122" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G11" s="234" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H11" s="235"/>
     </row>
@@ -37769,7 +37774,7 @@
         <v>2007.5</v>
       </c>
       <c r="C12" s="220" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="237" t="s">
@@ -37800,10 +37805,10 @@
         <v>134929.0</v>
       </c>
       <c r="B14" s="243" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C14" s="240" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="244" t="s">
@@ -37812,7 +37817,7 @@
       <c r="F14" s="161"/>
       <c r="G14" s="241"/>
       <c r="H14" s="245" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" ht="16.5" customHeight="1">
@@ -37823,7 +37828,7 @@
         <v>2021.7</v>
       </c>
       <c r="C15" s="240" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D15" s="116"/>
       <c r="E15" s="239" t="s">
@@ -37832,7 +37837,7 @@
       <c r="F15" s="248"/>
       <c r="G15" s="249"/>
       <c r="H15" s="245" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1">
@@ -37840,10 +37845,10 @@
         <v>456678.0</v>
       </c>
       <c r="B16" s="244" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C16" s="251" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D16" s="206">
         <v>96.0</v>
@@ -37854,7 +37859,7 @@
       <c r="F16" s="253"/>
       <c r="G16" s="254"/>
       <c r="H16" s="255" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" ht="16.5" customHeight="1">
@@ -37869,12 +37874,12 @@
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="259" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F17" s="153"/>
       <c r="G17" s="238"/>
       <c r="H17" s="221" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" ht="16.5" customHeight="1">
@@ -37885,14 +37890,14 @@
         <v>133</v>
       </c>
       <c r="C18" s="260" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="156"/>
       <c r="G18" s="238"/>
       <c r="H18" s="221" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" ht="16.5" customHeight="1">
@@ -37910,7 +37915,7 @@
       <c r="F19" s="262"/>
       <c r="G19" s="238"/>
       <c r="H19" s="221" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" ht="16.5" customHeight="1">
@@ -37928,7 +37933,7 @@
       <c r="F20" s="219"/>
       <c r="G20" s="238"/>
       <c r="H20" s="221" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" ht="16.5" customHeight="1">
@@ -37939,14 +37944,14 @@
         <v>2016.2</v>
       </c>
       <c r="C21" s="260" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="156"/>
       <c r="G21" s="238"/>
       <c r="H21" s="221" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" ht="16.5" customHeight="1">
@@ -37964,7 +37969,7 @@
       <c r="F22" s="261"/>
       <c r="G22" s="238"/>
       <c r="H22" s="245" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" ht="16.5" customHeight="1">
@@ -37972,7 +37977,7 @@
         <v>1.006506E7</v>
       </c>
       <c r="B23" s="264" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C23" s="265" t="s">
         <v>58</v>
@@ -37982,7 +37987,7 @@
       <c r="F23" s="261"/>
       <c r="G23" s="241"/>
       <c r="H23" s="221" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" ht="16.5" customHeight="1">
@@ -37993,14 +37998,14 @@
         <v>155</v>
       </c>
       <c r="C24" s="267" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D24" s="116"/>
       <c r="E24" s="116"/>
       <c r="F24" s="268"/>
       <c r="G24" s="249"/>
       <c r="H24" s="245" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I24" s="269"/>
     </row>
@@ -39035,13 +39040,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="276" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B1" s="276" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C1" s="276" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -39061,7 +39066,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="276" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -39088,47 +39093,47 @@
     <row r="1" ht="16.5" customHeight="1"/>
     <row r="2" ht="16.5" customHeight="1">
       <c r="B2" s="276" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="C3" s="276" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="C4" s="276" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
       <c r="C5" s="276" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1">
       <c r="C6" s="276" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="C7" s="276" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" ht="16.5" customHeight="1">
       <c r="C8" s="276" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" ht="16.5" customHeight="1">
       <c r="C9" s="276" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
       <c r="C10" s="276" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" ht="16.5" customHeight="1"/>

</xml_diff>